<commit_message>
chore(public/files): Replace contract template
</commit_message>
<xml_diff>
--- a/public/files/合同批量签署模板.xlsx
+++ b/public/files/合同批量签署模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6880"/>
+    <workbookView windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>姓名</t>
   </si>
@@ -22,32 +22,29 @@
     <t>身份证号</t>
   </si>
   <si>
-    <t>手机号码</t>
-  </si>
-  <si>
-    <t>合同开始时间</t>
-  </si>
-  <si>
-    <t>合同结束时间</t>
-  </si>
-  <si>
-    <t>张三</t>
-  </si>
-  <si>
-    <t>420114198204217025</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>签署日期</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="23">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -58,6 +55,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -205,6 +209,12 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -527,147 +537,150 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -989,53 +1002,34 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="15.6" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="17.1083333333333" customWidth="1"/>
     <col min="2" max="2" width="20.975" customWidth="1"/>
-    <col min="3" max="3" width="16.075" customWidth="1"/>
-    <col min="4" max="5" width="13.8333333333333" customWidth="1"/>
+    <col min="3" max="4" width="13.8333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>18717955345</v>
-      </c>
-      <c r="D2" s="2">
-        <v>45187</v>
-      </c>
-      <c r="E2" s="2">
-        <v>45553</v>
-      </c>
+    <row r="2" spans="3:4">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>

<commit_message>
chore: Update files template
</commit_message>
<xml_diff>
--- a/public/files/合同批量签署模板.xlsx
+++ b/public/files/合同批量签署模板.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11700"/>
+    <workbookView windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,23 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>姓名</t>
   </si>
   <si>
     <t>身份证号</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>签署日期</t>
-    </r>
   </si>
 </sst>
 </file>
@@ -44,7 +33,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -209,12 +198,6 @@
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1005,7 +988,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14166666666667" defaultRowHeight="15.6" outlineLevelRow="1" outlineLevelCol="3"/>
@@ -1022,9 +1005,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="C1" s="2"/>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="3:4">

</xml_diff>